<commit_message>
#84604 - Provider Submission Report added into 1920 periodend report service.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76811A44-A918-4CF7-B955-AEAACA1ADE4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD166CA-CACF-4474-A383-ABB5686DAF44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17790" yWindow="-16725" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ILR Provider Submissions Report" sheetId="4" r:id="rId1"/>
@@ -263,7 +263,7 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;No&quot;"/>
+      <numFmt numFmtId="166" formatCode=";;;&quot;No&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode=";;;&quot;Yes&quot;"/>
@@ -683,7 +683,7 @@
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.15234375" style="2"/>
-    <col min="2" max="2" width="23" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58.3828125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.69140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.53515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.84375" style="2" customWidth="1"/>

</xml_diff>

<commit_message>
#84604 - Provider submissions report code refactoring around getting latest files submitted, fixed the issues raised while running the app in service fabric and some report formatting done.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD166CA-CACF-4474-A383-ABB5686DAF44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E91E8B-8DAD-480F-B04D-CC892F8F725A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ILR Provider Submissions Report" sheetId="4" r:id="rId1"/>
@@ -212,7 +212,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -245,9 +245,6 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -677,26 +674,26 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="2"/>
-    <col min="2" max="2" width="58.3828125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.69140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.53515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.84375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.3828125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="58.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="14" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.84375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.3046875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.3046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.15234375" style="2"/>
+    <col min="11" max="11" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
@@ -711,7 +708,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
@@ -726,7 +723,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -739,7 +736,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
@@ -754,7 +751,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
@@ -769,7 +766,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
@@ -784,7 +781,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -799,7 +796,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
@@ -814,7 +811,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
@@ -829,7 +826,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -842,7 +839,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:12" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -874,11 +871,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="37.299999999999997" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="2:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="10" t="s">

</xml_diff>

<commit_message>
Updated templates to have different worksheet name to correct tests. Renamed the model lists in data quality to improve readability of the code.
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA50C50-2889-4204-9324-5005D3A1602B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BDA50C50-2889-4204-9324-5005D3A1602B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EBAB3BBA-BA00-4139-A369-744A9132E6EB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
+    <sheet name="Provider Submissions" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -114,8 +114,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -196,7 +196,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
@@ -215,7 +215,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -236,15 +236,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;&quot;No&quot;;&quot;Yes&quot;"/>
+      <numFmt numFmtId="168" formatCode=";;;&quot;No&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;Yes&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;No&quot;"/>
+      <numFmt numFmtId="167" formatCode=";;;&quot;Yes&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -651,26 +648,26 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.1328125" style="3"/>
     <col min="2" max="2" width="23" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.73046875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" style="3" customWidth="1"/>
     <col min="7" max="7" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.265625" style="3" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -685,7 +682,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -700,7 +697,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -713,7 +710,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
@@ -728,7 +725,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -743,7 +740,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
@@ -758,7 +755,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -773,7 +770,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -788,7 +785,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
@@ -803,7 +800,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -816,7 +813,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -848,7 +845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -885,7 +882,7 @@
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Uplifted internal reports to match POC, added valid aims report
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BDA50C50-2889-4204-9324-5005D3A1602B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EBAB3BBA-BA00-4139-A369-744A9132E6EB}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="113_{5040190B-C5AC-4B39-A761-840B4A5452A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62E556F1-CB9B-4E4E-AF9B-184CE00D241D}"/>
   <bookViews>
     <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Provider Submissions" sheetId="4" r:id="rId1"/>
+    <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Quality'!$B$12:$K$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -648,7 +651,7 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B12" sqref="B12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -878,6 +881,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B12:K12" xr:uid="{570F393E-551D-4C93-8A5E-417B7F021624}"/>
   <conditionalFormatting sqref="D13:E13">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>

</xml_diff>

<commit_message>
Correct worksheet name in template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
+++ b/src/ESFA.DC.PeriodEnd.ReportService.InternalReports/Assets/ProviderSubmissionsReportTemplate.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="113_{5040190B-C5AC-4B39-A761-840B4A5452A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{62E556F1-CB9B-4E4E-AF9B-184CE00D241D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058D3B93-638C-45C4-B4B4-781F5F094B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Quality" sheetId="4" r:id="rId1"/>
+    <sheet name="Provider Submissions" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Quality'!$B$12:$K$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Provider Submissions'!$B$12:$K$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -117,8 +117,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -199,7 +199,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
@@ -218,7 +218,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -241,10 +241,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;No&quot;"/>
+      <numFmt numFmtId="165" formatCode=";;;&quot;No&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Yes&quot;"/>
+      <numFmt numFmtId="166" formatCode=";;;&quot;Yes&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -651,26 +651,26 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:K12"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="23" style="3" customWidth="1"/>
-    <col min="3" max="3" width="51.73046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.3984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="11" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="3"/>
+    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -685,7 +685,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -713,7 +713,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
@@ -728,7 +728,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
@@ -743,7 +743,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
@@ -803,7 +803,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -816,7 +816,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" s="9" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>